<commit_message>
inserted data from set1
</commit_message>
<xml_diff>
--- a/Data Collection Sim 0.xlsx
+++ b/Data Collection Sim 0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umeer\Desktop\University\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB597327-A529-4813-9EEF-48287FCF36AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE3148B-1D26-4535-B148-7DB69C8C4AA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22608" yWindow="324" windowWidth="21600" windowHeight="11388" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="111">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -740,6 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -753,10 +754,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -764,7 +765,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
@@ -894,19 +894,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>8.6457818286992824E-2</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.10990855550168863</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.6036028556171878E-2</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.3177849229914702E-2</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.21854593017003399</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -918,19 +918,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>8.6457818286992824E-2</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.10990855550168863</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.6036028556171878E-2</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.3177849229914702E-2</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.21854593017003399</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -955,6 +955,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.406666666668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50833333333499997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61000000000200005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.828033901848002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.866405287816001</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>115.854555972505</c:v>
                 </c:pt>
@@ -19644,9 +19659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19721,7 +19736,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="4">
@@ -19743,7 +19758,7 @@
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
         <v>100</v>
@@ -19765,7 +19780,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -19785,7 +19800,7 @@
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
         <v>100</v>
@@ -19807,7 +19822,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -19827,7 +19842,7 @@
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
         <v>100</v>
@@ -19853,7 +19868,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -19873,7 +19888,7 @@
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>100</v>
@@ -19896,7 +19911,7 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -19917,7 +19932,7 @@
       </c>
       <c r="G6" s="35"/>
       <c r="H6" s="35">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I6" s="35">
         <v>100</v>
@@ -19942,7 +19957,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -19963,7 +19978,7 @@
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
         <v>100</v>
@@ -19988,7 +20003,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -20031,7 +20046,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="5">
@@ -20078,7 +20093,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -20123,7 +20138,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -20168,7 +20183,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -20211,7 +20226,7 @@
       <c r="T12" s="26"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="39" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="6">
@@ -20255,7 +20270,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -20297,7 +20312,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -20339,7 +20354,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -20381,7 +20396,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -20423,7 +20438,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -20510,7 +20525,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="40" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="20">
@@ -20557,7 +20572,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="20">
         <v>2</v>
       </c>
@@ -20602,7 +20617,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="37" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="10">
@@ -20646,7 +20661,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -20688,7 +20703,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -20730,7 +20745,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -20772,7 +20787,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -20814,7 +20829,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="37" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="12">
@@ -20861,7 +20876,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -20903,7 +20918,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -20945,7 +20960,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -20987,7 +21002,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -21029,7 +21044,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -21071,7 +21086,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B33" s="14">
@@ -21115,7 +21130,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -21157,7 +21172,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -21199,7 +21214,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -21241,7 +21256,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -21283,7 +21298,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="37" t="s">
         <v>108</v>
       </c>
       <c r="B38" s="23">
@@ -21324,7 +21339,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="23">
         <v>2</v>
       </c>
@@ -21363,7 +21378,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="23">
         <v>3</v>
       </c>
@@ -21402,7 +21417,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="23">
         <v>4</v>
       </c>
@@ -21441,7 +21456,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="23">
         <v>5</v>
       </c>
@@ -21480,7 +21495,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="37" t="s">
         <v>109</v>
       </c>
       <c r="B43" s="27">
@@ -21524,7 +21539,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="27">
         <v>2</v>
       </c>
@@ -21566,7 +21581,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="27">
         <v>3</v>
       </c>
@@ -21608,7 +21623,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="27">
         <v>4</v>
       </c>
@@ -21650,7 +21665,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
+      <c r="A47" s="37"/>
       <c r="B47" s="27">
         <v>5</v>
       </c>
@@ -21692,7 +21707,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
+      <c r="A48" s="37"/>
       <c r="B48" s="27">
         <v>6</v>
       </c>
@@ -21770,8 +21785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:X101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21807,36 +21822,71 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C2">
+        <v>18.630216736592001</v>
+      </c>
+      <c r="D2">
+        <v>35.646030341458001</v>
+      </c>
+      <c r="E2">
+        <v>2.017634968416</v>
+      </c>
+      <c r="F2">
+        <v>53.234294590434999</v>
+      </c>
       <c r="G2">
         <v>75.482852674233996</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>6.2723094744900001</v>
+      </c>
+      <c r="C3">
+        <v>58.191610608266998</v>
+      </c>
+      <c r="D3">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E3">
+        <v>38.851899188891998</v>
+      </c>
+      <c r="F3">
+        <v>49.409732583093998</v>
+      </c>
       <c r="G3">
         <v>108.358154340563</v>
       </c>
-      <c r="K3" s="18" t="s">
-        <v>63</v>
-      </c>
+      <c r="K3" s="18"/>
       <c r="L3" s="18"/>
-      <c r="N3" s="18" t="s">
-        <v>78</v>
-      </c>
+      <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="Q3" s="18" t="s">
-        <v>79</v>
-      </c>
+      <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
-      <c r="T3" s="18" t="s">
-        <v>80</v>
-      </c>
+      <c r="T3" s="18"/>
       <c r="U3" s="18"/>
-      <c r="W3" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="W3" s="18"/>
       <c r="X3" s="18"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>10.022588624299001</v>
+      </c>
+      <c r="C4">
+        <v>9.7453150162059998</v>
+      </c>
+      <c r="D4">
+        <v>45.886422461709998</v>
+      </c>
+      <c r="E4">
+        <v>32.189801913821</v>
+      </c>
+      <c r="F4">
+        <v>105.613371723786</v>
+      </c>
       <c r="G4">
         <v>182.33288944551299</v>
       </c>
@@ -21852,511 +21902,501 @@
       <c r="X4" s="16"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>6.1711102002729996</v>
+      </c>
+      <c r="C5">
+        <v>10.006929993511999</v>
+      </c>
+      <c r="D5">
+        <v>25.775478090671001</v>
+      </c>
+      <c r="E5">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F5">
+        <v>90.443172394396001</v>
+      </c>
       <c r="G5">
         <v>134.826828606639</v>
       </c>
-      <c r="K5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" s="16">
-        <v>0.65907088731205998</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="O5" s="16">
-        <v>0.96447097937686022</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="16">
-        <v>0.89090111111418024</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="U5" s="16">
-        <v>0.91610186017854023</v>
-      </c>
-      <c r="W5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="X5" s="16">
-        <v>1.0695115236070001</v>
-      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C6">
+        <v>0.813333333336</v>
+      </c>
+      <c r="D6">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E6">
+        <v>86.678416396144002</v>
+      </c>
+      <c r="F6">
+        <v>53.351097299393999</v>
+      </c>
       <c r="G6">
         <v>215.759151188153</v>
       </c>
-      <c r="K6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="16">
-        <v>4.3022931756713616E-2</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="O6" s="16">
-        <v>5.4692431251639792E-2</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" s="16">
-        <v>3.7836865796969356E-2</v>
-      </c>
-      <c r="T6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="U6" s="16">
-        <v>3.643300751720354E-2</v>
-      </c>
-      <c r="W6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="X6" s="16">
-        <v>8.5018079230275018E-2</v>
-      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C7">
+        <v>28.219820264641001</v>
+      </c>
+      <c r="D7">
+        <v>14.743895338495999</v>
+      </c>
+      <c r="E7">
+        <v>5.1432438142769996</v>
+      </c>
+      <c r="F7">
+        <v>140.19251694441201</v>
+      </c>
       <c r="G7">
         <v>201.88244572619999</v>
       </c>
-      <c r="K7" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="16">
-        <v>0.61020000000200003</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="O7" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="U7" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="W7" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="X7" s="16">
-        <v>0.97033335269749998</v>
-      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C8">
+        <v>15.686468596215001</v>
+      </c>
+      <c r="D8">
+        <v>10.220385744445</v>
+      </c>
+      <c r="E8">
+        <v>99.902198446400007</v>
+      </c>
+      <c r="F8">
+        <v>208.08815480700699</v>
+      </c>
       <c r="G8">
         <v>115.660653538319</v>
       </c>
-      <c r="K8" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="16">
-        <v>0.61020000000200003</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="T8" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="U8" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="W8" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="X8" s="16" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>16.178163874385</v>
+      </c>
+      <c r="C9">
+        <v>16.849180423155001</v>
+      </c>
+      <c r="D9">
+        <v>40.528470843210997</v>
+      </c>
+      <c r="E9">
+        <v>14.95461860432</v>
+      </c>
+      <c r="F9">
+        <v>145.55117584944199</v>
+      </c>
       <c r="G9">
         <v>116.45964582443101</v>
       </c>
-      <c r="K9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="16">
-        <v>0.30421806791698264</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="16">
-        <v>0.38673389017613552</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" s="16">
-        <v>0.26754704383882377</v>
-      </c>
-      <c r="T9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="U9" s="16">
-        <v>0.26018371562067272</v>
-      </c>
-      <c r="W9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="X9" s="16">
-        <v>0.20825091302568619</v>
-      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2.3075806218050001</v>
+      </c>
+      <c r="C10">
+        <v>28.803743387714</v>
+      </c>
+      <c r="D10">
+        <v>5.2213901449779998</v>
+      </c>
+      <c r="E10">
+        <v>12.322482975243</v>
+      </c>
+      <c r="F10">
+        <v>66.449024054437004</v>
+      </c>
       <c r="G10">
         <v>214.338102300846</v>
       </c>
-      <c r="K10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" s="16">
-        <v>9.2548632847141848E-2</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="O10" s="16">
-        <v>0.14956310181076726</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="R10" s="16">
-        <v>7.1581420666893478E-2</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="U10" s="16">
-        <v>6.7695565874179089E-2</v>
-      </c>
-      <c r="W10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="X10" s="16">
-        <v>4.3368442776031912E-2</v>
-      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C11">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D11">
+        <v>53.517206987061002</v>
+      </c>
+      <c r="E11">
+        <v>135.08107512120699</v>
+      </c>
+      <c r="F11">
+        <v>389.40241348158298</v>
+      </c>
       <c r="G11">
         <v>95.323242813232</v>
       </c>
-      <c r="K11" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11" s="16">
-        <v>-0.82635308083923675</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="O11" s="16">
-        <v>-0.39915931653301362</v>
-      </c>
-      <c r="Q11" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="R11" s="16">
-        <v>-0.5239911534935402</v>
-      </c>
-      <c r="T11" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="U11" s="16">
-        <v>1.0288759383420598</v>
-      </c>
-      <c r="W11" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="X11" s="16">
-        <v>0.33027136427514669</v>
-      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1.790981020289</v>
+      </c>
+      <c r="C12">
+        <v>42.431284081633997</v>
+      </c>
+      <c r="D12">
+        <v>15.308534080801</v>
+      </c>
+      <c r="E12">
+        <v>34.234056610229999</v>
+      </c>
+      <c r="F12">
+        <v>76.264945388626003</v>
+      </c>
       <c r="G12">
         <v>163.43124597162</v>
       </c>
-      <c r="K12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" s="16">
-        <v>0.43711523073040359</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="O12" s="16">
-        <v>0.31095602990822668</v>
-      </c>
-      <c r="Q12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="R12" s="16">
-        <v>-0.40775931790969783</v>
-      </c>
-      <c r="T12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U12" s="16">
-        <v>-0.17512408574241317</v>
-      </c>
-      <c r="W12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="X12" s="16">
-        <v>1.2772222108687623</v>
-      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>11.852762693120001</v>
+      </c>
+      <c r="C13">
+        <v>5.1967217058240003</v>
+      </c>
+      <c r="D13">
+        <v>30.240461067243</v>
+      </c>
+      <c r="E13">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F13">
+        <v>73.267128382492004</v>
+      </c>
       <c r="G13">
         <v>117.562326673806</v>
       </c>
-      <c r="K13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="L13" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="O13" s="16">
-        <v>1.5255000000050001</v>
-      </c>
-      <c r="Q13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="R13" s="16">
-        <v>0.91530000000300005</v>
-      </c>
-      <c r="T13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="U13" s="16">
-        <v>1.2455994742050001</v>
-      </c>
-      <c r="W13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="X13" s="16">
-        <v>0.50855585887099997</v>
-      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C14">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D14">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E14">
+        <v>93.239786180021994</v>
+      </c>
+      <c r="F14">
+        <v>151.64626054038399</v>
+      </c>
       <c r="G14">
         <v>435.54856523996898</v>
       </c>
-      <c r="K14" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" s="16">
-        <v>0.30510000000100002</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="O14" s="16">
-        <v>0.30510000000100002</v>
-      </c>
-      <c r="Q14" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="R14" s="16">
-        <v>0.30510000000100002</v>
-      </c>
-      <c r="T14" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="U14" s="16">
-        <v>0.30510000000100002</v>
-      </c>
-      <c r="W14" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="X14" s="16">
-        <v>0.91530000000300005</v>
-      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C15">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="D15">
+        <v>50.762691352498003</v>
+      </c>
+      <c r="E15">
+        <v>88.032491808649993</v>
+      </c>
+      <c r="F15">
+        <v>61.565601037690001</v>
+      </c>
       <c r="G15">
         <v>46.524248721147998</v>
       </c>
-      <c r="K15" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="L15" s="16">
-        <v>1.2204000000040001</v>
-      </c>
-      <c r="N15" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="O15" s="16">
-        <v>1.8306000000060001</v>
-      </c>
-      <c r="Q15" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="R15" s="16">
-        <v>1.2204000000040001</v>
-      </c>
-      <c r="T15" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="U15" s="16">
-        <v>1.5506994742060001</v>
-      </c>
-      <c r="W15" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="X15" s="16">
-        <v>1.423855858874</v>
-      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C16">
+        <v>20.341581331705001</v>
+      </c>
+      <c r="D16">
+        <v>2.3616569438770001</v>
+      </c>
+      <c r="E16">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="F16">
+        <v>160.53775245733601</v>
+      </c>
       <c r="G16">
         <v>588.61394135668604</v>
       </c>
-      <c r="K16" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="L16" s="16">
-        <v>32.953544365603001</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="O16" s="16">
-        <v>48.223548968843012</v>
-      </c>
-      <c r="Q16" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="R16" s="16">
-        <v>44.545055555709013</v>
-      </c>
-      <c r="T16" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="U16" s="16">
-        <v>46.721194869105553</v>
-      </c>
-      <c r="W16" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="X16" s="16">
-        <v>6.417069141642</v>
-      </c>
-    </row>
-    <row r="17" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>6.7155947364059996</v>
+      </c>
+      <c r="C17">
+        <v>9.9173101424630001</v>
+      </c>
+      <c r="D17">
+        <v>23.807568475250999</v>
+      </c>
+      <c r="E17">
+        <v>0.406666666668</v>
+      </c>
+      <c r="F17">
+        <v>76.005560091909004</v>
+      </c>
       <c r="G17">
         <v>86.702755354393005</v>
       </c>
-      <c r="K17" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="16">
-        <v>50</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="O17" s="16">
-        <v>50</v>
-      </c>
-      <c r="Q17" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="R17" s="16">
-        <v>50</v>
-      </c>
-      <c r="T17" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="U17" s="16">
-        <v>51</v>
-      </c>
-      <c r="W17" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="X17" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="7:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+    </row>
+    <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C18">
+        <v>15.776328544798</v>
+      </c>
+      <c r="D18">
+        <v>8.7768883371289999</v>
+      </c>
+      <c r="E18">
+        <v>0.406666666668</v>
+      </c>
+      <c r="F18">
+        <v>56.813917909552998</v>
+      </c>
       <c r="G18">
         <v>371.494373231042</v>
       </c>
-      <c r="K18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" s="17">
-        <v>8.6457818286992824E-2</v>
-      </c>
-      <c r="N18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="O18" s="17">
-        <v>0.10990855550168863</v>
-      </c>
-      <c r="Q18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="R18" s="17">
-        <v>7.6036028556171878E-2</v>
-      </c>
-      <c r="T18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="U18" s="17">
-        <v>7.3177849229914702E-2</v>
-      </c>
-      <c r="W18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="X18" s="17">
-        <v>0.21854593017003399</v>
-      </c>
-    </row>
-    <row r="19" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="C19">
+        <v>7.7012001663670002</v>
+      </c>
+      <c r="D19">
+        <v>25.970025448255999</v>
+      </c>
+      <c r="E19">
+        <v>55.385629338127998</v>
+      </c>
+      <c r="F19">
+        <v>7.4971940956639997</v>
+      </c>
       <c r="G19">
         <v>53.380889609467999</v>
       </c>
     </row>
-    <row r="20" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>15.813796946996</v>
+      </c>
+      <c r="C20">
+        <v>21.572917702659002</v>
+      </c>
+      <c r="D20">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E20">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="F20">
+        <v>14.219324660766</v>
+      </c>
       <c r="G20">
         <v>441.640206569876</v>
       </c>
     </row>
-    <row r="21" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C21">
+        <v>10.524888052398</v>
+      </c>
+      <c r="D21">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E21">
+        <v>60.784065727992001</v>
+      </c>
+      <c r="F21">
+        <v>43.725170471479998</v>
+      </c>
       <c r="G21">
         <v>147.34377417589499</v>
       </c>
     </row>
-    <row r="22" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>13.149058738736001</v>
+      </c>
+      <c r="C22">
+        <v>13.348530938972999</v>
+      </c>
+      <c r="D22">
+        <v>51.855878885644998</v>
+      </c>
+      <c r="E22">
+        <v>14.612284331521</v>
+      </c>
+      <c r="F22">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="G22">
         <v>64.966739072569993</v>
       </c>
@@ -22365,26 +22405,41 @@
       </c>
       <c r="L22">
         <f>L5</f>
-        <v>0.65907088731205998</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <f>O5</f>
-        <v>0.96447097937686022</v>
+        <v>0</v>
       </c>
       <c r="N22">
         <f>R5</f>
-        <v>0.89090111111418024</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <f>U5</f>
-        <v>0.91610186017854023</v>
+        <v>0</v>
       </c>
       <c r="P22">
         <f>X5</f>
-        <v>1.0695115236070001</v>
-      </c>
-    </row>
-    <row r="23" spans="7:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C23">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="D23">
+        <v>46.226278601761997</v>
+      </c>
+      <c r="E23">
+        <v>55.035831453221</v>
+      </c>
+      <c r="F23">
+        <v>179.57046674866399</v>
+      </c>
       <c r="G23">
         <v>262.57309033228199</v>
       </c>
@@ -22393,106 +22448,361 @@
       </c>
       <c r="L23">
         <f>L18</f>
-        <v>8.6457818286992824E-2</v>
+        <v>0</v>
       </c>
       <c r="M23">
         <f>O18</f>
-        <v>0.10990855550168863</v>
+        <v>0</v>
       </c>
       <c r="N23">
         <f>R18</f>
-        <v>7.6036028556171878E-2</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <f>U18</f>
-        <v>7.3177849229914702E-2</v>
+        <v>0</v>
       </c>
       <c r="P23">
         <f>X18</f>
-        <v>0.21854593017003399</v>
-      </c>
-    </row>
-    <row r="24" spans="7:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C24">
+        <v>3.0773594512739999</v>
+      </c>
+      <c r="D24">
+        <v>80.334750690036998</v>
+      </c>
+      <c r="E24">
+        <v>104.966962879142</v>
+      </c>
+      <c r="F24">
+        <v>54.839811899147001</v>
+      </c>
       <c r="G24">
         <v>260.701079649885</v>
       </c>
     </row>
-    <row r="25" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>13.628518918738999</v>
+      </c>
+      <c r="C25">
+        <v>0.813333333336</v>
+      </c>
+      <c r="D25">
+        <v>12.960339769165</v>
+      </c>
+      <c r="E25">
+        <v>14.050312684707</v>
+      </c>
+      <c r="F25">
+        <v>158.66350859622801</v>
+      </c>
       <c r="G25">
         <v>120.64841159722501</v>
       </c>
     </row>
-    <row r="26" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C26">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D26">
+        <v>8.5650022037079996</v>
+      </c>
+      <c r="E26">
+        <v>49.402259132040001</v>
+      </c>
+      <c r="F26">
+        <v>110.45840160613101</v>
+      </c>
       <c r="G26">
         <v>164.653638178172</v>
       </c>
     </row>
-    <row r="27" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C27">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="D27">
+        <v>3.7794625148900001</v>
+      </c>
+      <c r="E27">
+        <v>0.85086366647800005</v>
+      </c>
+      <c r="F27">
+        <v>337.01645515801698</v>
+      </c>
       <c r="G27">
         <v>115.59407029974</v>
       </c>
     </row>
-    <row r="28" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C28">
+        <v>1.8958130776990001</v>
+      </c>
+      <c r="D28">
+        <v>10.143536666481999</v>
+      </c>
+      <c r="E28">
+        <v>78.551389718409993</v>
+      </c>
+      <c r="F28">
+        <v>226.35979097149399</v>
+      </c>
       <c r="G28">
         <v>77.676793094409007</v>
       </c>
     </row>
-    <row r="29" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="C29">
+        <v>13.750286921562999</v>
+      </c>
+      <c r="D29">
+        <v>107.76835999182801</v>
+      </c>
+      <c r="E29">
+        <v>47.080276112619998</v>
+      </c>
+      <c r="F29">
+        <v>231.37397312938299</v>
+      </c>
       <c r="G29">
         <v>282.365223872554</v>
       </c>
     </row>
-    <row r="30" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C30">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D30">
+        <v>64.501893789644001</v>
+      </c>
+      <c r="E30">
+        <v>10.356834578100001</v>
+      </c>
+      <c r="F30">
+        <v>308.637935324907</v>
+      </c>
       <c r="G30">
         <v>134.894126575325</v>
       </c>
     </row>
-    <row r="31" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C31">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="D31">
+        <v>8.0230139579860005</v>
+      </c>
+      <c r="E31">
+        <v>70.493163274188007</v>
+      </c>
+      <c r="F31">
+        <v>223.359500721579</v>
+      </c>
       <c r="G31">
         <v>126.128342579772</v>
       </c>
     </row>
-    <row r="32" spans="7:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>12.566321005895</v>
+      </c>
+      <c r="C32">
+        <v>9.3917785379200005</v>
+      </c>
+      <c r="D32">
+        <v>34.661248041557002</v>
+      </c>
+      <c r="E32">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="F32">
+        <v>122.29022536406301</v>
+      </c>
       <c r="G32">
         <v>190.97008897622601</v>
       </c>
     </row>
-    <row r="33" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C33">
+        <v>3.9777059603780001</v>
+      </c>
+      <c r="D33">
+        <v>12.312182290934</v>
+      </c>
+      <c r="E33">
+        <v>91.141451755036996</v>
+      </c>
+      <c r="F33">
+        <v>182.08811610357799</v>
+      </c>
       <c r="G33">
         <v>204.982459897572</v>
       </c>
     </row>
-    <row r="34" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C34">
+        <v>0.80131862141200005</v>
+      </c>
+      <c r="D34">
+        <v>47.672577787601</v>
+      </c>
+      <c r="E34">
+        <v>68.391172737231997</v>
+      </c>
+      <c r="F34">
+        <v>5.6670126139699999</v>
+      </c>
       <c r="G34">
         <v>411.15462886416498</v>
       </c>
     </row>
-    <row r="35" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C35">
+        <v>20.240164638707</v>
+      </c>
+      <c r="D35">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E35">
+        <v>29.443943973707</v>
+      </c>
+      <c r="F35">
+        <v>48.434060473237999</v>
+      </c>
       <c r="G35">
         <v>22.688487693548002</v>
       </c>
     </row>
-    <row r="36" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C36">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D36">
+        <v>31.903574607446998</v>
+      </c>
+      <c r="E36">
+        <v>29.058959529380001</v>
+      </c>
+      <c r="F36">
+        <v>259.65207564902602</v>
+      </c>
       <c r="G36">
         <v>295.39638831480602</v>
       </c>
     </row>
-    <row r="37" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>3.417796444226</v>
+      </c>
+      <c r="C37">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D37">
+        <v>14.064698701208</v>
+      </c>
+      <c r="E37">
+        <v>22.927914661347</v>
+      </c>
+      <c r="F37">
+        <v>27.077655481322001</v>
+      </c>
       <c r="G37">
         <v>196.269730307527</v>
       </c>
     </row>
-    <row r="38" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="C38">
+        <v>1.642784973256</v>
+      </c>
+      <c r="D38">
+        <v>1.1402242782959999</v>
+      </c>
+      <c r="E38">
+        <v>98.133645956587998</v>
+      </c>
+      <c r="F38">
+        <v>169.327713796251</v>
+      </c>
       <c r="G38">
         <v>67.683320258291005</v>
       </c>
     </row>
-    <row r="39" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C39">
+        <v>11.217654902465</v>
+      </c>
+      <c r="D39">
+        <v>41.276105001452002</v>
+      </c>
+      <c r="E39">
+        <v>27.486369322375001</v>
+      </c>
+      <c r="F39">
+        <v>232.437417917342</v>
+      </c>
       <c r="G39">
         <v>481.74514624923103</v>
       </c>
     </row>
-    <row r="40" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D40">
+        <v>12.396113908497</v>
+      </c>
+      <c r="E40">
+        <v>66.704918341953004</v>
+      </c>
+      <c r="F40">
+        <v>207.945435994154</v>
+      </c>
       <c r="G40">
         <v>207.027740624659</v>
       </c>
@@ -22506,27 +22816,57 @@
       <c r="O40" s="41"/>
       <c r="P40" s="41"/>
     </row>
-    <row r="41" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C41">
+        <v>26.311338851361999</v>
+      </c>
+      <c r="D41">
+        <v>94.348887372787004</v>
+      </c>
+      <c r="E41">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F41">
+        <v>157.00499740959199</v>
+      </c>
       <c r="G41">
         <v>71.942921234606004</v>
       </c>
       <c r="J41" t="s">
         <v>106</v>
       </c>
-      <c r="K41" s="40" t="s">
+      <c r="K41" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40" t="s">
+      <c r="L41" s="42"/>
+      <c r="M41" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="N41" s="40"/>
-      <c r="O41" s="40" t="s">
+      <c r="N41" s="42"/>
+      <c r="O41" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="P41" s="40"/>
-    </row>
-    <row r="42" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="P41" s="42"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C42">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D42">
+        <v>34.398073949134002</v>
+      </c>
+      <c r="E42">
+        <v>8.1036945923159998</v>
+      </c>
+      <c r="F42">
+        <v>187.67635807960701</v>
+      </c>
       <c r="G42">
         <v>324.92483404370103</v>
       </c>
@@ -22536,20 +22876,35 @@
       <c r="J42">
         <v>10</v>
       </c>
-      <c r="K42" s="40">
+      <c r="K42" s="42">
         <v>1.2</v>
       </c>
-      <c r="L42" s="40"/>
-      <c r="M42" s="40">
+      <c r="L42" s="42"/>
+      <c r="M42" s="42">
         <v>3</v>
       </c>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40">
+      <c r="N42" s="42"/>
+      <c r="O42" s="42">
         <v>1.7929999999999999</v>
       </c>
-      <c r="P42" s="40"/>
-    </row>
-    <row r="43" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="P42" s="42"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C43">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="D43">
+        <v>3.681030360906</v>
+      </c>
+      <c r="E43">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F43">
+        <v>189.447032811795</v>
+      </c>
       <c r="G43">
         <v>128.518617588659</v>
       </c>
@@ -22559,20 +22914,35 @@
       <c r="J43">
         <v>20</v>
       </c>
-      <c r="K43" s="40">
+      <c r="K43" s="42">
         <v>1.3</v>
       </c>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40">
+      <c r="L43" s="42"/>
+      <c r="M43" s="42">
         <v>4</v>
       </c>
-      <c r="N43" s="40"/>
-      <c r="O43" s="40">
+      <c r="N43" s="42"/>
+      <c r="O43" s="42">
         <v>1.8839999999999999</v>
       </c>
-      <c r="P43" s="40"/>
-    </row>
-    <row r="44" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="P43" s="42"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C44">
+        <v>22.362417966672002</v>
+      </c>
+      <c r="D44">
+        <v>6.7095269162099997</v>
+      </c>
+      <c r="E44">
+        <v>50.169120227364999</v>
+      </c>
+      <c r="F44">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="G44">
         <v>275.09504881078601</v>
       </c>
@@ -22582,20 +22952,35 @@
       <c r="J44">
         <v>50</v>
       </c>
-      <c r="K44" s="40">
+      <c r="K44" s="42">
         <v>2.36</v>
       </c>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40">
+      <c r="L44" s="42"/>
+      <c r="M44" s="42">
         <v>6</v>
       </c>
-      <c r="N44" s="40"/>
-      <c r="O44" s="40">
+      <c r="N44" s="42"/>
+      <c r="O44" s="42">
         <v>2.2669999999999999</v>
       </c>
-      <c r="P44" s="40"/>
-    </row>
-    <row r="45" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="P44" s="42"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C45">
+        <v>10.365486463657</v>
+      </c>
+      <c r="D45">
+        <v>42.47405737687</v>
+      </c>
+      <c r="E45">
+        <v>11.926744215447</v>
+      </c>
+      <c r="F45">
+        <v>314.63395171376902</v>
+      </c>
       <c r="G45">
         <v>195.13322084120099</v>
       </c>
@@ -22605,20 +22990,35 @@
       <c r="J45">
         <v>100</v>
       </c>
-      <c r="K45" s="40">
+      <c r="K45" s="42">
         <v>2.5499999999999998</v>
       </c>
-      <c r="L45" s="40"/>
-      <c r="M45" s="40">
+      <c r="L45" s="42"/>
+      <c r="M45" s="42">
         <v>8</v>
       </c>
-      <c r="N45" s="40"/>
-      <c r="O45" s="40">
+      <c r="N45" s="42"/>
+      <c r="O45" s="42">
         <v>2.8820000000000001</v>
       </c>
-      <c r="P45" s="40"/>
-    </row>
-    <row r="46" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="P45" s="42"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>17.537941040911999</v>
+      </c>
+      <c r="C46">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D46">
+        <v>7.4722401705749997</v>
+      </c>
+      <c r="E46">
+        <v>45.461697130087003</v>
+      </c>
+      <c r="F46">
+        <v>118.165601526559</v>
+      </c>
       <c r="G46">
         <v>103.63792642895901</v>
       </c>
@@ -22626,303 +23026,1138 @@
         <v>5</v>
       </c>
       <c r="J46">
-        <v>1000</v>
-      </c>
-      <c r="K46" s="40">
-        <v>3.55</v>
-      </c>
-      <c r="L46" s="40"/>
-      <c r="M46" s="40">
-        <v>12</v>
-      </c>
-      <c r="N46" s="40"/>
-      <c r="O46" s="40">
-        <v>4.1079999999999997</v>
-      </c>
-      <c r="P46" s="40"/>
-    </row>
-    <row r="47" spans="7:16" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
+      <c r="N46" s="42"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="42"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>9.5244459912400004</v>
+      </c>
+      <c r="C47">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D47">
+        <v>46.830036201094003</v>
+      </c>
+      <c r="E47">
+        <v>5.4967324627469996</v>
+      </c>
+      <c r="F47">
+        <v>1302.67897561985</v>
+      </c>
       <c r="G47">
         <v>392.30318056909198</v>
       </c>
-    </row>
-    <row r="48" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>6</v>
+      </c>
+      <c r="J47">
+        <v>1000</v>
+      </c>
+      <c r="K47" s="42">
+        <v>3.55</v>
+      </c>
+      <c r="L47" s="42"/>
+      <c r="M47" s="42">
+        <v>12</v>
+      </c>
+      <c r="N47" s="42"/>
+      <c r="O47" s="42">
+        <v>4.1079999999999997</v>
+      </c>
+      <c r="P47" s="42"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C48">
+        <v>0.813333333336</v>
+      </c>
+      <c r="D48">
+        <v>6.8869318531810002</v>
+      </c>
+      <c r="E48">
+        <v>0.406666666668</v>
+      </c>
+      <c r="F48">
+        <v>153.149673265225</v>
+      </c>
       <c r="G48">
         <v>468.89023599369398</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C49">
+        <v>59.545461078955</v>
+      </c>
+      <c r="D49">
+        <v>62.247861208944002</v>
+      </c>
+      <c r="E49">
+        <v>2.9302375280150001</v>
+      </c>
+      <c r="F49">
+        <v>442.62012148203502</v>
+      </c>
       <c r="G49">
         <v>140.42318825362801</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C50">
+        <v>7.3452239308719998</v>
+      </c>
+      <c r="D50">
+        <v>0.406666666668</v>
+      </c>
+      <c r="E50">
+        <v>25.729634938137</v>
+      </c>
+      <c r="F50">
+        <v>189.13909790722801</v>
+      </c>
       <c r="G50">
         <v>341.09450125046197</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>3.5233421995329999</v>
+      </c>
+      <c r="C51">
+        <v>17.915116336406999</v>
+      </c>
+      <c r="D51">
+        <v>26.157284725164001</v>
+      </c>
+      <c r="E51">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F51">
+        <v>106.372294121343</v>
+      </c>
       <c r="G51">
         <v>214.36813919517701</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="44">
+      <c r="B52" s="36">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C52" s="36">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D52" s="36">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E52" s="36">
+        <v>41.828033901848002</v>
+      </c>
+      <c r="F52" s="36">
+        <v>30.866405287816001</v>
+      </c>
+      <c r="G52" s="36">
         <v>115.854555972505</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C53">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D53">
+        <v>3.6525900079600002</v>
+      </c>
+      <c r="E53">
+        <v>8.4869592579069995</v>
+      </c>
+      <c r="F53">
+        <v>173.78884682533101</v>
+      </c>
       <c r="G53">
         <v>311.38048194408901</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C54">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D54">
+        <v>42.794862011120998</v>
+      </c>
+      <c r="E54">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="F54">
+        <v>53.888007384237</v>
+      </c>
       <c r="G54">
         <v>107.47033688200599</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>28.322210376009998</v>
+      </c>
+      <c r="C55">
+        <v>32.432763678287003</v>
+      </c>
+      <c r="D55">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E55">
+        <v>31.526809550206</v>
+      </c>
+      <c r="F55">
+        <v>253.48141695486299</v>
+      </c>
       <c r="G55">
         <v>295.04579862025003</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>27.809751662490999</v>
+      </c>
+      <c r="C56">
+        <v>23.683399378238001</v>
+      </c>
+      <c r="D56">
+        <v>28.901100303155001</v>
+      </c>
+      <c r="E56">
+        <v>64.081744579146999</v>
+      </c>
+      <c r="F56">
+        <v>155.891540592121</v>
+      </c>
       <c r="G56">
         <v>3.055973270285</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C57">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D57">
+        <v>3.8078333522840002</v>
+      </c>
+      <c r="E57">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F57">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="G57">
         <v>99.205916725045995</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>3.1754842850010001</v>
+      </c>
+      <c r="C58">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D58">
+        <v>18.490176486488998</v>
+      </c>
+      <c r="E58">
+        <v>90.349248236993006</v>
+      </c>
+      <c r="F58">
+        <v>0.406666666668</v>
+      </c>
       <c r="G58">
         <v>263.19777591765398</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>17.894892719017001</v>
+      </c>
+      <c r="C59">
+        <v>18.799200739968999</v>
+      </c>
+      <c r="D59">
+        <v>25.470006288337999</v>
+      </c>
+      <c r="E59">
+        <v>7.7532099889249997</v>
+      </c>
+      <c r="F59">
+        <v>164.146706085304</v>
+      </c>
       <c r="G59">
         <v>202.957194341264</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C60">
+        <v>39.724344413708998</v>
+      </c>
+      <c r="D60">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E60">
+        <v>15.165855163454999</v>
+      </c>
+      <c r="F60">
+        <v>149.34735163230201</v>
+      </c>
       <c r="G60">
         <v>78.929086700659994</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C61">
+        <v>21.341151289687001</v>
+      </c>
+      <c r="D61">
+        <v>5.0052666023599999</v>
+      </c>
+      <c r="E61">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F61">
+        <v>55.052370049334002</v>
+      </c>
       <c r="G61">
         <v>301.96342502124202</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>25.536257904770999</v>
+      </c>
+      <c r="C62">
+        <v>27.865843604169999</v>
+      </c>
+      <c r="D62">
+        <v>8.7763741247650007</v>
+      </c>
+      <c r="E62">
+        <v>35.134066048754001</v>
+      </c>
+      <c r="F62">
+        <v>37.81482370618</v>
+      </c>
       <c r="G62">
         <v>443.934189927565</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>5.2325084226829999</v>
+      </c>
+      <c r="C63">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D63">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E63">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F63">
+        <v>103.266934573328</v>
+      </c>
       <c r="G63">
         <v>0.71166666666900003</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C64">
+        <v>1.7756344105670001</v>
+      </c>
+      <c r="D64">
+        <v>68.854258470421001</v>
+      </c>
+      <c r="E64">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F64">
+        <v>39.426595874773</v>
+      </c>
       <c r="G64">
         <v>47.417512654692999</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>14.148977555778</v>
+      </c>
+      <c r="C65">
+        <v>32.996631678706002</v>
+      </c>
+      <c r="D65">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E65">
+        <v>56.818761986863002</v>
+      </c>
+      <c r="F65">
+        <v>124.815934206805</v>
+      </c>
       <c r="G65">
         <v>177.61986579333299</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>14.827911043217</v>
+      </c>
+      <c r="C66">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D66">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E66">
+        <v>88.725614065017993</v>
+      </c>
+      <c r="F66">
+        <v>177.318650824147</v>
+      </c>
       <c r="G66">
         <v>93.278348153707995</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>30.125507783187999</v>
+      </c>
+      <c r="C67">
+        <v>4.519549277636</v>
+      </c>
+      <c r="D67">
+        <v>81.829584711904999</v>
+      </c>
+      <c r="E67">
+        <v>0.813333333336</v>
+      </c>
+      <c r="F67">
+        <v>0.50833333333499997</v>
+      </c>
       <c r="G67">
         <v>283.78541313224599</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>11.198646520606999</v>
+      </c>
+      <c r="C68">
+        <v>24.974899266764002</v>
+      </c>
+      <c r="D68">
+        <v>27.720717295587999</v>
+      </c>
+      <c r="E68">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F68">
+        <v>91.250895492612003</v>
+      </c>
       <c r="G68">
         <v>219.40371542928801</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="C69">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D69">
+        <v>0.406666666668</v>
+      </c>
+      <c r="E69">
+        <v>33.320327124472001</v>
+      </c>
+      <c r="F69">
+        <v>75.026065635375005</v>
+      </c>
       <c r="G69">
         <v>376.2210226103</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C70">
+        <v>5.3565661213610003</v>
+      </c>
+      <c r="D70">
+        <v>85.136094657689995</v>
+      </c>
+      <c r="E70">
+        <v>133.77686629561001</v>
+      </c>
+      <c r="F70">
+        <v>315.860003630091</v>
+      </c>
       <c r="G70">
         <v>314.15390649384398</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>13.097642643453</v>
+      </c>
+      <c r="C71">
+        <v>31.850320021752001</v>
+      </c>
+      <c r="D71">
+        <v>6.5316745823240003</v>
+      </c>
+      <c r="E71">
+        <v>42.710353006630001</v>
+      </c>
+      <c r="F71">
+        <v>99.573468666034998</v>
+      </c>
       <c r="G71">
         <v>182.259932613026</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C72">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="D72">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E72">
+        <v>65.934921739535</v>
+      </c>
+      <c r="F72">
+        <v>179.70039621088301</v>
+      </c>
       <c r="G72">
         <v>75.965647347065001</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>2.9572546207469999</v>
+      </c>
+      <c r="C73">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D73">
+        <v>0.406666666668</v>
+      </c>
+      <c r="E73">
+        <v>133.90524144655899</v>
+      </c>
+      <c r="F73">
+        <v>39.395036768280001</v>
+      </c>
       <c r="G73">
         <v>138.47957172017399</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C74">
+        <v>5.5938936934520003</v>
+      </c>
+      <c r="D74">
+        <v>0.406666666668</v>
+      </c>
+      <c r="E74">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="F74">
+        <v>411.92036090321801</v>
+      </c>
       <c r="G74">
         <v>32.985180864497003</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C75">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D75">
+        <v>8.3321253846429997</v>
+      </c>
+      <c r="E75">
+        <v>10.457213951599</v>
+      </c>
+      <c r="F75">
+        <v>32.675111561336003</v>
+      </c>
       <c r="G75">
         <v>52.283042254028999</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C76">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="D76">
+        <v>23.264753694509999</v>
+      </c>
+      <c r="E76">
+        <v>68.601784589185002</v>
+      </c>
+      <c r="F76">
+        <v>12.684328270424</v>
+      </c>
       <c r="G76">
         <v>142.03301635017399</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>15.282793612827</v>
+      </c>
+      <c r="C77">
+        <v>33.662477846629002</v>
+      </c>
+      <c r="D77">
+        <v>33.504995070573997</v>
+      </c>
+      <c r="E77">
+        <v>6.0328862674519996</v>
+      </c>
+      <c r="F77">
+        <v>105.75258597056801</v>
+      </c>
       <c r="G77">
         <v>61.174649477480003</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C78">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D78">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E78">
+        <v>41.015323147727003</v>
+      </c>
+      <c r="F78">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="G78">
         <v>401.78510693407998</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C79">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="D79">
+        <v>27.115507758166999</v>
+      </c>
+      <c r="E79">
+        <v>33.037804756626002</v>
+      </c>
+      <c r="F79">
+        <v>49.281173927485</v>
+      </c>
       <c r="G79">
         <v>231.43576988547301</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="C80">
+        <v>23.369941937244</v>
+      </c>
+      <c r="D80">
+        <v>23.332949398703001</v>
+      </c>
+      <c r="E80">
+        <v>42.862706986501998</v>
+      </c>
+      <c r="F80">
+        <v>553.62445485001399</v>
+      </c>
       <c r="G80">
         <v>24.953089168097002</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>17.316442666589001</v>
+      </c>
+      <c r="C81">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D81">
+        <v>9.4408969463550001</v>
+      </c>
+      <c r="E81">
+        <v>47.174483146531003</v>
+      </c>
+      <c r="F81">
+        <v>107.07785055682</v>
+      </c>
       <c r="G81">
         <v>0.71166666666900003</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C82">
+        <v>44.160456998043998</v>
+      </c>
+      <c r="D82">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E82">
+        <v>25.116995861267</v>
+      </c>
+      <c r="F82">
+        <v>449.57333035797399</v>
+      </c>
       <c r="G82">
         <v>59.881119630809003</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>8.153544472159</v>
+      </c>
+      <c r="C83">
+        <v>6.6858184850270002</v>
+      </c>
+      <c r="D83">
+        <v>55.892516086074998</v>
+      </c>
+      <c r="E83">
+        <v>32.026899080286</v>
+      </c>
+      <c r="F83">
+        <v>337.71606921770598</v>
+      </c>
       <c r="G83">
         <v>345.89987002363802</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C84">
+        <v>5.3583797948539997</v>
+      </c>
+      <c r="D84">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="E84">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F84">
+        <v>181.660310234843</v>
+      </c>
       <c r="G84">
         <v>165.960000483644</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>19.317744104003999</v>
+      </c>
+      <c r="C85">
+        <v>12.481648125594999</v>
+      </c>
+      <c r="D85">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E85">
+        <v>1.107539585402</v>
+      </c>
+      <c r="F85">
+        <v>51.100849885039999</v>
+      </c>
       <c r="G85">
         <v>145.161502339658</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>17.931334004119002</v>
+      </c>
+      <c r="C86">
+        <v>26.594614915558999</v>
+      </c>
+      <c r="D86">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E86">
+        <v>163.53766131592499</v>
+      </c>
+      <c r="F86">
+        <v>0.50833333333499997</v>
+      </c>
       <c r="G86">
         <v>801.43765520804095</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C87">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D87">
+        <v>0.406666666668</v>
+      </c>
+      <c r="E87">
+        <v>27.168449220248</v>
+      </c>
+      <c r="F87">
+        <v>315.45075756115</v>
+      </c>
       <c r="G87">
         <v>384.53817500556602</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>17.202081044985999</v>
+      </c>
+      <c r="C88">
+        <v>13.764683748976999</v>
+      </c>
+      <c r="D88">
+        <v>17.648199632476999</v>
+      </c>
+      <c r="E88">
+        <v>20.240172224165001</v>
+      </c>
+      <c r="F88">
+        <v>0.813333333336</v>
+      </c>
       <c r="G88">
         <v>316.37321431914899</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C89">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D89">
+        <v>20.185488745080999</v>
+      </c>
+      <c r="E89">
+        <v>53.250527466560001</v>
+      </c>
+      <c r="F89">
+        <v>189.485584745278</v>
+      </c>
       <c r="G89">
         <v>127.668943016612</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C90">
+        <v>36.012511863526001</v>
+      </c>
+      <c r="D90">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E90">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F90">
+        <v>129.74032361631299</v>
+      </c>
       <c r="G90">
         <v>135.35760747539999</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>19.972905360919</v>
+      </c>
+      <c r="C91">
+        <v>16.367203281140998</v>
+      </c>
+      <c r="D91">
+        <v>30.371796016198001</v>
+      </c>
+      <c r="E91">
+        <v>4.0926055180540004</v>
+      </c>
+      <c r="F91">
+        <v>215.364158086088</v>
+      </c>
       <c r="G91">
         <v>88.123859268858993</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>22.00863899738</v>
+      </c>
+      <c r="C92">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D92">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E92">
+        <v>40.657853564261003</v>
+      </c>
+      <c r="F92">
+        <v>197.840756446185</v>
+      </c>
       <c r="G92">
         <v>0.71166666666900003</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C93">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="D93">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="E93">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="F93">
+        <v>54.241083684918003</v>
+      </c>
       <c r="G93">
         <v>96.344996679432001</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C94">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D94">
+        <v>11.435585365942</v>
+      </c>
+      <c r="E94">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="F94">
+        <v>80.303317444178006</v>
+      </c>
       <c r="G94">
         <v>124.10372662862299</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>19.914338772327</v>
+      </c>
+      <c r="C95">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="D95">
+        <v>13.610883230456</v>
+      </c>
+      <c r="E95">
+        <v>24.964190793105999</v>
+      </c>
+      <c r="F95">
+        <v>77.959665146901003</v>
+      </c>
       <c r="G95">
         <v>187.07135795687401</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>0.30500000000100003</v>
+      </c>
+      <c r="C96">
+        <v>4.8676845187279998</v>
+      </c>
+      <c r="D96">
+        <v>21.304633273355002</v>
+      </c>
+      <c r="E96">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="F96">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="G96">
         <v>89.927449309771006</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C97">
+        <v>17.993565606901001</v>
+      </c>
+      <c r="D97">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E97">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="F97">
+        <v>76.015944812027001</v>
+      </c>
       <c r="G97">
         <v>506.78310102983698</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C98">
+        <v>21.095186196099998</v>
+      </c>
+      <c r="D98">
+        <v>67.728811746912996</v>
+      </c>
+      <c r="E98">
+        <v>5.0725625826030001</v>
+      </c>
+      <c r="F98">
+        <v>96.232015236256998</v>
+      </c>
       <c r="G98">
         <v>128.014113039694</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C99">
+        <v>6.7231223498460002</v>
+      </c>
+      <c r="D99">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E99">
+        <v>83.485358655252</v>
+      </c>
       <c r="G99">
         <v>20.745411063750002</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C100">
+        <v>9.583215006903</v>
+      </c>
+      <c r="D100">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E100">
+        <v>79.193221262807995</v>
+      </c>
       <c r="G100">
         <v>66.971189478723005</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>21.172210518517002</v>
+      </c>
+      <c r="C101">
+        <v>17.804098621731001</v>
+      </c>
+      <c r="D101">
+        <v>15.837311987010001</v>
+      </c>
+      <c r="E101">
+        <v>63.126462498484997</v>
+      </c>
       <c r="G101">
         <v>193.39721661619399</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="O46:P46"/>
     <mergeCell ref="J40:P40"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="K44:L44"/>
@@ -22933,15 +24168,6 @@
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="M42:N42"/>
     <mergeCell ref="O42:P42"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="O43:P43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -44150,7 +45376,7 @@
       </c>
     </row>
     <row r="108" spans="1:26" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="42" t="s">
+      <c r="A108" s="43" t="s">
         <v>109</v>
       </c>
       <c r="B108" s="5">
@@ -44173,7 +45399,7 @@
       </c>
     </row>
     <row r="109" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="43"/>
+      <c r="A109" s="44"/>
       <c r="B109">
         <v>1.32</v>
       </c>
@@ -44218,7 +45444,7 @@
       <c r="Z109" s="18"/>
     </row>
     <row r="110" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="43"/>
+      <c r="A110" s="44"/>
       <c r="B110">
         <v>4.9858304269760003</v>
       </c>
@@ -44251,7 +45477,7 @@
       <c r="Z110" s="16"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A111" s="43"/>
+      <c r="A111" s="44"/>
       <c r="B111">
         <v>6.3728169473809997</v>
       </c>
@@ -44308,7 +45534,7 @@
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A112" s="43"/>
+      <c r="A112" s="44"/>
       <c r="B112">
         <v>9.3210768256519998</v>
       </c>

</xml_diff>

<commit_message>
inserted data from test 9 (sim0)
</commit_message>
<xml_diff>
--- a/Data Collection Sim 0.xlsx
+++ b/Data Collection Sim 0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umeer\Desktop\University\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE186371-2955-4D74-A177-1F52675EAF1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B06EF97-E21E-4DFA-8B25-7C716AB27DFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -344,10 +344,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="#,##0.000000000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
+    <numFmt numFmtId="183" formatCode="0.00000000000"/>
+    <numFmt numFmtId="184" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -590,7 +593,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,9 +606,10 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -675,20 +679,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="12" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="12" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="13" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="13" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="13"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="60% - Accent1" xfId="10" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="11" builtinId="36"/>
     <cellStyle name="60% - Accent4" xfId="9" builtinId="44"/>
@@ -696,7 +702,8 @@
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53"/>
+    <cellStyle name="Comma" xfId="12" builtinId="3"/>
+    <cellStyle name="Explanatory Text" xfId="13" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
@@ -18639,8 +18646,8 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33:A37"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20795,10 +20802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
-  <dimension ref="A1:P101"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23003,6 +23010,32 @@
       </c>
       <c r="G101">
         <v>193.39721661619399</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="7">
+        <f>AVERAGE(B2:B101)</f>
+        <v>5.5214805828889588</v>
+      </c>
+      <c r="C102" s="7">
+        <f>AVERAGE(C2:C101)</f>
+        <v>11.33199432943567</v>
+      </c>
+      <c r="D102" s="7">
+        <f t="shared" ref="C102:G102" si="0">AVERAGE(D2:D101)</f>
+        <v>21.109886040443318</v>
+      </c>
+      <c r="E102" s="7">
+        <f t="shared" si="0"/>
+        <v>35.235011978285819</v>
+      </c>
+      <c r="F102" s="7">
+        <f t="shared" si="0"/>
+        <v>102.54954653965635</v>
+      </c>
+      <c r="G102" s="7">
+        <f t="shared" si="0"/>
+        <v>193.21242648788314</v>
       </c>
     </row>
   </sheetData>
@@ -23037,10 +23070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8ADDF3-F6DC-49DE-90F6-6F07047D1F12}">
-  <dimension ref="A1:Q1001"/>
+  <dimension ref="A1:Q1002"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A166" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24570,6 +24603,10 @@
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="7">
+        <f>AVERAGE(B2:B101)</f>
+        <v>102.54954653965635</v>
+      </c>
       <c r="C102" s="28">
         <v>256.03348630134798</v>
       </c>
@@ -25428,6 +25465,10 @@
       </c>
     </row>
     <row r="180" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C180" s="7">
+        <f>AVERAGE(C2:C179)</f>
+        <v>123.92416126226949</v>
+      </c>
       <c r="D180" s="28">
         <v>45.716699041277003</v>
       </c>
@@ -30261,6 +30302,12 @@
     <row r="1001" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D1001" s="28">
         <v>145.09921649036701</v>
+      </c>
+    </row>
+    <row r="1002" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1002" s="7">
+        <f>AVERAGE(D2:D1001)</f>
+        <v>125.89198592564668</v>
       </c>
     </row>
   </sheetData>
@@ -30271,10 +30318,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB14316-39CC-412C-A762-31F37CE381A2}">
-  <dimension ref="A1:P101"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32358,6 +32405,32 @@
       </c>
       <c r="G101">
         <v>100.53117275410899</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="7">
+        <f>AVERAGE(B2:B101)</f>
+        <v>567.52936722291315</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" ref="C102:G102" si="0">AVERAGE(C2:C101)</f>
+        <v>137.32851215026486</v>
+      </c>
+      <c r="D102" s="7">
+        <f t="shared" si="0"/>
+        <v>115.46403979834899</v>
+      </c>
+      <c r="E102" s="7">
+        <f t="shared" si="0"/>
+        <v>116.4595298035816</v>
+      </c>
+      <c r="F102" s="7">
+        <f t="shared" si="0"/>
+        <v>121.47862956712029</v>
+      </c>
+      <c r="G102" s="7">
+        <f t="shared" si="0"/>
+        <v>125.75558301610687</v>
       </c>
     </row>
   </sheetData>
@@ -42637,8 +42710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEB8E32-D847-46DD-A9C2-FCA6CC8CF645}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="R96" sqref="R96"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44413,11 +44486,26 @@
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B102" s="28"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
+      <c r="B102" s="7">
+        <f>AVERAGE(B2:B101)</f>
+        <v>98.811194611377999</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" ref="C102:F102" si="0">AVERAGE(C2:C101)</f>
+        <v>109.30226050461641</v>
+      </c>
+      <c r="D102" s="7">
+        <f t="shared" si="0"/>
+        <v>102.54954653965635</v>
+      </c>
+      <c r="E102" s="7">
+        <f t="shared" si="0"/>
+        <v>450.71714130953342</v>
+      </c>
+      <c r="F102" s="7">
+        <f t="shared" si="0"/>
+        <v>16191.786017132834</v>
+      </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="28"/>
@@ -44436,8 +44524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE560BB-010F-4538-8606-72D35C2079F1}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46452,7 +46540,9 @@
       <c r="D98" s="28">
         <v>50.517302127724001</v>
       </c>
-      <c r="E98" s="28"/>
+      <c r="E98" s="28">
+        <v>206.68521586864199</v>
+      </c>
       <c r="F98" s="28">
         <v>183.63746924976499</v>
       </c>
@@ -46470,7 +46560,9 @@
       <c r="D99" s="28">
         <v>36.000054616729997</v>
       </c>
-      <c r="E99" s="28"/>
+      <c r="E99" s="28">
+        <v>118.297081984106</v>
+      </c>
       <c r="F99" s="28">
         <v>146.13459715412199</v>
       </c>
@@ -46485,8 +46577,12 @@
       <c r="C100" s="28">
         <v>67.081683671850996</v>
       </c>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
+      <c r="D100" s="28">
+        <v>182.372494086247</v>
+      </c>
+      <c r="E100" s="28">
+        <v>98.854456549424995</v>
+      </c>
       <c r="F100" s="28">
         <v>0.61016666666800001</v>
       </c>
@@ -46501,8 +46597,12 @@
       <c r="C101" s="28">
         <v>110.12879755426</v>
       </c>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
+      <c r="D101" s="28">
+        <v>125.78557982594801</v>
+      </c>
+      <c r="E101" s="28">
+        <v>46.777544888016998</v>
+      </c>
       <c r="F101" s="28">
         <v>27.749304471230001</v>
       </c>
@@ -46511,12 +46611,30 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B102" s="28"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
-      <c r="G102" s="28"/>
+      <c r="B102" s="7">
+        <f>AVERAGE(B2:B101)</f>
+        <v>102.54954653965635</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" ref="C102:G102" si="0">AVERAGE(C2:C101)</f>
+        <v>118.89658364760797</v>
+      </c>
+      <c r="D102" s="7">
+        <f t="shared" si="0"/>
+        <v>118.41586913425608</v>
+      </c>
+      <c r="E102" s="7">
+        <f>AVERAGE(E2:E101)</f>
+        <v>98.372853389724511</v>
+      </c>
+      <c r="F102" s="7">
+        <f t="shared" si="0"/>
+        <v>126.80498435993009</v>
+      </c>
+      <c r="G102" s="7">
+        <f t="shared" si="0"/>
+        <v>118.45145669079341</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B103" s="28"/>
@@ -46554,8 +46672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB00259A-76EF-42CC-A63F-F0BB8151E029}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48330,11 +48448,26 @@
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B102" s="28"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
+      <c r="B102" s="7">
+        <f>AVERAGE(B2:B101)</f>
+        <v>108.52063876400031</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" ref="C102:F102" si="0">AVERAGE(C2:C101)</f>
+        <v>41.359168470417529</v>
+      </c>
+      <c r="D102" s="7">
+        <f t="shared" si="0"/>
+        <v>251.66183465383642</v>
+      </c>
+      <c r="E102" s="7">
+        <f t="shared" si="0"/>
+        <v>1836.8521270775389</v>
+      </c>
+      <c r="F102" s="7">
+        <f t="shared" si="0"/>
+        <v>22960.01355553676</v>
+      </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="28"/>
@@ -48417,16 +48550,16 @@
   <dimension ref="A1:AA105"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -48452,165 +48585,365 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
+      <c r="B2" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C2" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D2" s="40">
+        <v>87.436393806940998</v>
+      </c>
+      <c r="E2" s="41">
+        <v>250.09296160712199</v>
+      </c>
+      <c r="F2" s="43">
+        <v>655.28547836164603</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="B3" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C3" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D3" s="40">
+        <v>184.578324422208</v>
+      </c>
+      <c r="E3" s="41">
+        <v>55.696932691256002</v>
+      </c>
+      <c r="F3" s="43">
+        <v>4087.1148103248602</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="B4" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C4" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D4" s="40">
+        <v>210.840393233296</v>
+      </c>
+      <c r="E4" s="41">
+        <v>176.45556663527199</v>
+      </c>
+      <c r="F4" s="43">
+        <v>4126.67146411467</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
+      <c r="B5" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C5" s="40">
+        <v>110.311281170382</v>
+      </c>
+      <c r="D5" s="40">
+        <v>45.27214752135</v>
+      </c>
+      <c r="E5" s="41">
+        <v>312.73053741213101</v>
+      </c>
+      <c r="F5" s="43">
+        <v>2379.3352547640902</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="42"/>
+      <c r="B6" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C6" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D6" s="40">
+        <v>66.634162536689004</v>
+      </c>
+      <c r="E6" s="41">
+        <v>63.651510017919001</v>
+      </c>
+      <c r="F6" s="43">
+        <v>4154.4538241390001</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
+      <c r="B7" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C7" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D7" s="40">
+        <v>154.614846213524</v>
+      </c>
+      <c r="E7" s="41">
+        <v>58.960814161080002</v>
+      </c>
+      <c r="F7" s="43">
+        <v>2607.6981729571398</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
+      <c r="B8" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C8" s="40">
+        <v>113.15620945111</v>
+      </c>
+      <c r="D8" s="40">
+        <v>222.67954919611799</v>
+      </c>
+      <c r="E8" s="41">
+        <v>7.6642678499479997</v>
+      </c>
+      <c r="F8" s="43">
+        <v>5308.2221052776604</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="42"/>
+      <c r="B9" s="44">
+        <v>0.406666666668</v>
+      </c>
+      <c r="C9" s="40">
+        <v>33.696513207873998</v>
+      </c>
+      <c r="D9" s="40">
+        <v>78.599566052674007</v>
+      </c>
+      <c r="E9" s="41">
+        <v>178.823888662808</v>
+      </c>
+      <c r="F9" s="43">
+        <v>421.980966458328</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="28"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
+      <c r="C10" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D10" s="40">
+        <v>30.642872555421999</v>
+      </c>
+      <c r="E10" s="41">
+        <v>226.64794878262501</v>
+      </c>
+      <c r="F10" s="43">
+        <v>4195.1749899176102</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="28"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42"/>
+      <c r="C11" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D11" s="40">
+        <v>1.2604497537929999</v>
+      </c>
+      <c r="E11" s="41">
+        <v>331.05062641088699</v>
+      </c>
+      <c r="F11" s="43">
+        <v>3997.7461100102901</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="28"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
+      <c r="C12" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D12" s="40">
+        <v>33.360520638086001</v>
+      </c>
+      <c r="E12" s="41">
+        <v>260.81205845457703</v>
+      </c>
+      <c r="F12" s="43">
+        <v>2892.65018454244</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
+      <c r="C13" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D13" s="40">
+        <v>131.14995814922</v>
+      </c>
+      <c r="E13" s="41">
+        <v>60.590890876339003</v>
+      </c>
+      <c r="F13" s="43">
+        <v>4880.8893986461899</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="28"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
+      <c r="C14" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D14" s="40">
+        <v>103.456745708874</v>
+      </c>
+      <c r="E14" s="41">
+        <v>67.381188754283997</v>
+      </c>
+      <c r="F14" s="43">
+        <v>2678.1647008825298</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="28"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
+      <c r="C15" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D15" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E15" s="41">
+        <v>92.636252996430002</v>
+      </c>
+      <c r="F15" s="43">
+        <v>734.86927591021401</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="28"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="42"/>
+      <c r="C16" s="40">
+        <v>95.678212007157001</v>
+      </c>
+      <c r="D16" s="40">
+        <v>122.452699723423</v>
+      </c>
+      <c r="E16" s="41">
+        <v>175.928690668314</v>
+      </c>
+      <c r="F16" s="43">
+        <v>2099.8203003578301</v>
+      </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="28"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="42"/>
+      <c r="C17" s="40">
+        <v>75.810779305322995</v>
+      </c>
+      <c r="D17" s="40">
+        <v>114.265521586603</v>
+      </c>
+      <c r="E17" s="41">
+        <v>311.64399519077398</v>
+      </c>
+      <c r="F17" s="43">
+        <v>2422.8303138598799</v>
+      </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" s="28"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42"/>
+      <c r="C18" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D18" s="40">
+        <v>267.82792769581198</v>
+      </c>
+      <c r="E18" s="41">
+        <v>237.544772872142</v>
+      </c>
+      <c r="F18" s="43">
+        <v>8054.5788923947503</v>
+      </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B19" s="28"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="42"/>
+      <c r="C19" s="40">
+        <v>156.30260621395999</v>
+      </c>
+      <c r="D19" s="40">
+        <v>29.170763040049</v>
+      </c>
+      <c r="E19" s="41">
+        <v>69.098917665715007</v>
+      </c>
+      <c r="F19" s="43">
+        <v>3713.7577391128102</v>
+      </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B20" s="28"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="42"/>
+      <c r="C20" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D20" s="40">
+        <v>163.51303762204799</v>
+      </c>
+      <c r="E20" s="41">
+        <v>331.541508233554</v>
+      </c>
+      <c r="F20" s="43">
+        <v>2031.06967010057</v>
+      </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" s="28"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42"/>
+      <c r="C21" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D21" s="40">
+        <v>92.559133586751997</v>
+      </c>
+      <c r="E21" s="41">
+        <v>1.4233333333380001</v>
+      </c>
+      <c r="F21" s="43">
+        <v>7.8785933977629998</v>
+      </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B22" s="28"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
+      <c r="C22" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D22" s="40">
+        <v>254.23426845159</v>
+      </c>
+      <c r="E22" s="41">
+        <v>125.415347195034</v>
+      </c>
+      <c r="F22" s="43">
+        <v>2927.0111982560502</v>
+      </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B23" s="28"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
+      <c r="C23" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D23" s="40">
+        <v>108.34635403481001</v>
+      </c>
+      <c r="E23" s="41">
+        <v>247.44443087251699</v>
+      </c>
+      <c r="F23" s="43">
+        <v>1154.48513568609</v>
+      </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B24" s="28"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
+      <c r="C24" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D24" s="40">
+        <v>149.418054453536</v>
+      </c>
+      <c r="E24" s="41">
+        <v>450.43177651501497</v>
+      </c>
+      <c r="F24" s="43">
+        <v>5292.7913587865996</v>
+      </c>
       <c r="I24" s="7" t="s">
         <v>29</v>
       </c>
@@ -48637,10 +48970,18 @@
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B25" s="28"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="42"/>
+      <c r="C25" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D25" s="40">
+        <v>390.43292197448199</v>
+      </c>
+      <c r="E25" s="41">
+        <v>202.774813275837</v>
+      </c>
+      <c r="F25" s="43">
+        <v>1850.03033107396</v>
+      </c>
       <c r="I25" s="7" t="s">
         <v>66</v>
       </c>
@@ -48667,537 +49008,1145 @@
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B26" s="28"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
+      <c r="C26" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D26" s="40">
+        <v>159.12073768594101</v>
+      </c>
+      <c r="E26" s="41">
+        <v>1.869123941042</v>
+      </c>
+      <c r="F26" s="43">
+        <v>2370.6722244738098</v>
+      </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B27" s="28"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
+      <c r="C27" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D27" s="40">
+        <v>57.327654570245002</v>
+      </c>
+      <c r="E27" s="41">
+        <v>103.713345870952</v>
+      </c>
+      <c r="F27" s="43">
+        <v>2810.0929567343601</v>
+      </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B28" s="28"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="42"/>
+      <c r="C28" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D28" s="40">
+        <v>159.73447435938201</v>
+      </c>
+      <c r="E28" s="41">
+        <v>228.507179525846</v>
+      </c>
+      <c r="F28" s="43">
+        <v>2225.1921827911001</v>
+      </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" s="28"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="42"/>
+      <c r="C29" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D29" s="40">
+        <v>65.396935537176006</v>
+      </c>
+      <c r="E29" s="41">
+        <v>58.829873000219003</v>
+      </c>
+      <c r="F29" s="43">
+        <v>3096.2313912260302</v>
+      </c>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B30" s="28"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="42"/>
+      <c r="C30" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D30" s="40">
+        <v>179.77448834887099</v>
+      </c>
+      <c r="E30" s="41">
+        <v>180.65286971922001</v>
+      </c>
+      <c r="F30" s="43">
+        <v>2886.7431009427401</v>
+      </c>
       <c r="AA30" s="7"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B31" s="28"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
+      <c r="C31" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D31" s="40">
+        <v>102.06707372027699</v>
+      </c>
+      <c r="E31" s="41">
+        <v>241.85561063503201</v>
+      </c>
+      <c r="F31" s="43">
+        <v>1742.6170603466801</v>
+      </c>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B32" s="28"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="42"/>
+      <c r="C32" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D32" s="40">
+        <v>292.23414330366597</v>
+      </c>
+      <c r="E32" s="41">
+        <v>45.062121172440001</v>
+      </c>
+      <c r="F32" s="43">
+        <v>2123.1560622004299</v>
+      </c>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" s="28"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="42"/>
+      <c r="C33" s="40">
+        <v>153.79980291901001</v>
+      </c>
+      <c r="D33" s="40">
+        <v>138.59695510659699</v>
+      </c>
+      <c r="E33" s="41">
+        <v>68.347284915651997</v>
+      </c>
+      <c r="F33" s="43">
+        <v>4128.2440344019096</v>
+      </c>
       <c r="Z33" s="7"/>
     </row>
     <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B34" s="28"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="42"/>
+      <c r="C34" s="40">
+        <v>33.080808019609997</v>
+      </c>
+      <c r="D34" s="40">
+        <v>192.082001447236</v>
+      </c>
+      <c r="E34" s="41">
+        <v>193.37227307137101</v>
+      </c>
+      <c r="F34" s="43">
+        <v>1135.95549166859</v>
+      </c>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B35" s="28"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="42"/>
+      <c r="C35" s="40">
+        <v>139.01642215807999</v>
+      </c>
+      <c r="D35" s="40">
+        <v>87.079367786887005</v>
+      </c>
+      <c r="E35" s="41">
+        <v>62.668967548863002</v>
+      </c>
+      <c r="F35" s="43">
+        <v>6382.5814739291</v>
+      </c>
     </row>
     <row r="36" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B36" s="28"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="42"/>
+      <c r="C36" s="40">
+        <v>165.38132297555299</v>
+      </c>
+      <c r="D36" s="40">
+        <v>350.46075987571902</v>
+      </c>
+      <c r="E36" s="41">
+        <v>160.592284817208</v>
+      </c>
+      <c r="F36" s="43">
+        <v>2765.6378439320702</v>
+      </c>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B37" s="28"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="42"/>
+      <c r="C37" s="40">
+        <v>27.276247497960998</v>
+      </c>
+      <c r="D37" s="40">
+        <v>96.707607369485999</v>
+      </c>
+      <c r="E37" s="41">
+        <v>203.54471560762201</v>
+      </c>
+      <c r="F37" s="43">
+        <v>1203.99849465992</v>
+      </c>
     </row>
     <row r="38" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B38" s="28"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="42"/>
+      <c r="C38" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D38" s="40">
+        <v>132.34025657224399</v>
+      </c>
+      <c r="E38" s="41">
+        <v>285.53796812001599</v>
+      </c>
+      <c r="F38" s="43">
+        <v>7627.2637157008103</v>
+      </c>
     </row>
     <row r="39" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B39" s="28"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="42"/>
+      <c r="C39" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D39" s="40">
+        <v>100.673930564828</v>
+      </c>
+      <c r="E39" s="41">
+        <v>44.883748065223003</v>
+      </c>
+      <c r="F39" s="43">
+        <v>3473.1528015333301</v>
+      </c>
     </row>
     <row r="40" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B40" s="28"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="42"/>
+      <c r="C40" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D40" s="40">
+        <v>23.392576793202</v>
+      </c>
+      <c r="E40" s="41">
+        <v>18.948177587288999</v>
+      </c>
+      <c r="F40" s="43">
+        <v>7012.3444669861801</v>
+      </c>
     </row>
     <row r="41" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B41" s="28"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="42"/>
+      <c r="C41" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D41" s="40">
+        <v>9.4883244944590004</v>
+      </c>
+      <c r="E41" s="41">
+        <v>26.610409123435002</v>
+      </c>
+      <c r="F41" s="43">
+        <v>3687.4077049841499</v>
+      </c>
     </row>
     <row r="42" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B42" s="28"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="42"/>
+      <c r="C42" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D42" s="40">
+        <v>43.243367125485001</v>
+      </c>
+      <c r="E42" s="41">
+        <v>217.11260618006301</v>
+      </c>
+      <c r="F42" s="43">
+        <v>2080.6288466138399</v>
+      </c>
     </row>
     <row r="43" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B43" s="28"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="42"/>
+      <c r="C43" s="40">
+        <v>29.114383458519001</v>
+      </c>
+      <c r="D43" s="40">
+        <v>187.66047127968</v>
+      </c>
+      <c r="E43" s="41">
+        <v>486.27978324303001</v>
+      </c>
+      <c r="F43" s="43">
+        <v>2514.4847605986702</v>
+      </c>
     </row>
     <row r="44" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B44" s="28"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="42"/>
+      <c r="C44" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D44" s="40">
+        <v>93.229633595729993</v>
+      </c>
+      <c r="E44" s="41">
+        <v>17.165649838421</v>
+      </c>
+      <c r="F44" s="43">
+        <v>2979.8627679695601</v>
+      </c>
     </row>
     <row r="45" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B45" s="28"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="42"/>
+      <c r="C45" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D45" s="40">
+        <v>98.316455384400001</v>
+      </c>
+      <c r="E45" s="41">
+        <v>42.336813207393</v>
+      </c>
+      <c r="F45" s="43">
+        <v>3458.8443913226401</v>
+      </c>
     </row>
     <row r="46" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B46" s="28"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="42"/>
+      <c r="C46" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D46" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E46" s="41">
+        <v>89.368656622892004</v>
+      </c>
+      <c r="F46" s="43">
+        <v>4095.55832394044</v>
+      </c>
     </row>
     <row r="47" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B47" s="28"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="42"/>
+      <c r="C47" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D47" s="40">
+        <v>168.68094039041301</v>
+      </c>
+      <c r="E47" s="41">
+        <v>246.72222946520799</v>
+      </c>
+      <c r="F47" s="43">
+        <v>2371.80893852598</v>
+      </c>
     </row>
     <row r="48" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B48" s="28"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="42"/>
+      <c r="C48" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D48" s="40">
+        <v>78.345589668257006</v>
+      </c>
+      <c r="E48" s="41">
+        <v>48.312987006352998</v>
+      </c>
+      <c r="F48" s="43">
+        <v>6907.4395345430803</v>
+      </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="28"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="42"/>
+      <c r="C49" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D49" s="40">
+        <v>217.34648769064199</v>
+      </c>
+      <c r="E49" s="41">
+        <v>308.21663687047999</v>
+      </c>
+      <c r="F49" s="43">
+        <v>2905.9726518110601</v>
+      </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="28"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="42"/>
+      <c r="C50" s="40">
+        <v>36.520098581325001</v>
+      </c>
+      <c r="D50" s="40">
+        <v>275.172064415298</v>
+      </c>
+      <c r="E50" s="41">
+        <v>201.253160983881</v>
+      </c>
+      <c r="F50" s="43">
+        <v>5541.0234249015502</v>
+      </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="28"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="42"/>
+      <c r="C51" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D51" s="40">
+        <v>212.13283379601901</v>
+      </c>
+      <c r="E51" s="41">
+        <v>54.685188476924999</v>
+      </c>
+      <c r="F51" s="43">
+        <v>792.72936076353596</v>
+      </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="28"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="42"/>
+      <c r="C52" s="40">
+        <v>90.695243929312994</v>
+      </c>
+      <c r="D52" s="40">
+        <v>41.633552105234997</v>
+      </c>
+      <c r="E52" s="41">
+        <v>26.806216322171998</v>
+      </c>
+      <c r="F52" s="43">
+        <v>5438.8241270082599</v>
+      </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="28"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="42"/>
+      <c r="C53" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D53" s="40">
+        <v>346.83149631235</v>
+      </c>
+      <c r="E53" s="41">
+        <v>228.02306232203401</v>
+      </c>
+      <c r="F53" s="43">
+        <v>2229.15504523241</v>
+      </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="28"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="42"/>
+      <c r="C54" s="40">
+        <v>8.7504044233790008</v>
+      </c>
+      <c r="D54" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E54" s="41">
+        <v>235.32672677198201</v>
+      </c>
+      <c r="F54" s="43">
+        <v>3751.85422799669</v>
+      </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="28"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="42"/>
+      <c r="C55" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D55" s="40">
+        <v>301.05274376500199</v>
+      </c>
+      <c r="E55" s="41">
+        <v>310.09662801133197</v>
+      </c>
+      <c r="F55" s="43">
+        <v>1489.3892495702401</v>
+      </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="28"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="42"/>
+      <c r="C56" s="40">
+        <v>17.281824381831999</v>
+      </c>
+      <c r="D56" s="40">
+        <v>164.86065254410701</v>
+      </c>
+      <c r="E56" s="41">
+        <v>240.852616602317</v>
+      </c>
+      <c r="F56" s="43">
+        <v>5983.97725011492</v>
+      </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="28"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="42"/>
+      <c r="C57" s="40">
+        <v>21.895567771024002</v>
+      </c>
+      <c r="D57" s="40">
+        <v>84.232411402142006</v>
+      </c>
+      <c r="E57" s="41">
+        <v>349.10961030841099</v>
+      </c>
+      <c r="F57" s="43">
+        <v>6543.6093282750899</v>
+      </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="28"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="42"/>
+      <c r="C58" s="40">
+        <v>10.290950251851999</v>
+      </c>
+      <c r="D58" s="40">
+        <v>204.69723998669701</v>
+      </c>
+      <c r="E58" s="41">
+        <v>77.922086064850006</v>
+      </c>
+      <c r="F58" s="43">
+        <v>3771.9574561715799</v>
+      </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="28"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="42"/>
+      <c r="C59" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D59" s="40">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="E59" s="41">
+        <v>14.058580287155999</v>
+      </c>
+      <c r="F59" s="43">
+        <v>3852.9891165434801</v>
+      </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="28"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="40"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="42"/>
+      <c r="C60" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D60" s="40">
+        <v>25.602510144421998</v>
+      </c>
+      <c r="E60" s="41">
+        <v>168.83822412216099</v>
+      </c>
+      <c r="F60" s="43">
+        <v>3264.7917319743101</v>
+      </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="28"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="41"/>
-      <c r="F61" s="42"/>
+      <c r="C61" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D61" s="40">
+        <v>69.608278180317001</v>
+      </c>
+      <c r="E61" s="41">
+        <v>57.163282007802998</v>
+      </c>
+      <c r="F61" s="43">
+        <v>695.92837218624004</v>
+      </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="28"/>
-      <c r="C62" s="40"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="41"/>
-      <c r="F62" s="42"/>
+      <c r="C62" s="40">
+        <v>117.28995565932399</v>
+      </c>
+      <c r="D62" s="40">
+        <v>122.436734944256</v>
+      </c>
+      <c r="E62" s="41">
+        <v>304.77454297791201</v>
+      </c>
+      <c r="F62" s="43">
+        <v>3529.5778640594799</v>
+      </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="28"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="41"/>
-      <c r="F63" s="42"/>
+      <c r="C63" s="40">
+        <v>29.335971849366</v>
+      </c>
+      <c r="D63" s="40">
+        <v>150.77137249215701</v>
+      </c>
+      <c r="E63" s="41">
+        <v>161.266628170844</v>
+      </c>
+      <c r="F63" s="43">
+        <v>1116.8966241974999</v>
+      </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="28"/>
-      <c r="C64" s="40"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="41"/>
-      <c r="F64" s="42"/>
+      <c r="C64" s="40">
+        <v>9.8452909244650009</v>
+      </c>
+      <c r="D64" s="40">
+        <v>239.11206143872101</v>
+      </c>
+      <c r="E64" s="41">
+        <v>325.27277851690599</v>
+      </c>
+      <c r="F64" s="43">
+        <v>6400.5787856557699</v>
+      </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="28"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="41"/>
-      <c r="F65" s="42"/>
+      <c r="C65" s="40">
+        <v>46.093754464973998</v>
+      </c>
+      <c r="D65" s="40">
+        <v>93.461166907220004</v>
+      </c>
+      <c r="E65" s="41">
+        <v>262.29572541806499</v>
+      </c>
+      <c r="F65" s="43">
+        <v>4901.2338346490696</v>
+      </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="28"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="42"/>
+      <c r="C66" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D66" s="40">
+        <v>33.184923596975999</v>
+      </c>
+      <c r="E66" s="41">
+        <v>326.306459269919</v>
+      </c>
+      <c r="F66" s="43">
+        <v>2648.9125019302601</v>
+      </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="28"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="42"/>
+      <c r="C67" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D67" s="40">
+        <v>91.176421038499001</v>
+      </c>
+      <c r="E67" s="41">
+        <v>85.435987863907997</v>
+      </c>
+      <c r="F67" s="43">
+        <v>5445.0791761617802</v>
+      </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="28"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="42"/>
+      <c r="C68" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D68" s="40">
+        <v>91.065492005061003</v>
+      </c>
+      <c r="E68" s="41">
+        <v>247.942279875613</v>
+      </c>
+      <c r="F68" s="43">
+        <v>6224.7203521389802</v>
+      </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="28"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="41"/>
-      <c r="F69" s="42"/>
+      <c r="C69" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D69" s="40">
+        <v>134.386109513279</v>
+      </c>
+      <c r="E69" s="41">
+        <v>405.30184326887598</v>
+      </c>
+      <c r="F69" s="43">
+        <v>2791.2688629979698</v>
+      </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="28"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="42"/>
+      <c r="C70" s="40">
+        <v>18.923516381075999</v>
+      </c>
+      <c r="D70" s="40">
+        <v>267.47069715822403</v>
+      </c>
+      <c r="E70" s="41">
+        <v>184.12642942779601</v>
+      </c>
+      <c r="F70" s="43">
+        <v>1177.20020121977</v>
+      </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="28"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="41"/>
-      <c r="F71" s="42"/>
+      <c r="C71" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D71" s="40">
+        <v>263.71545774104902</v>
+      </c>
+      <c r="E71" s="41">
+        <v>177.51290945812701</v>
+      </c>
+      <c r="F71" s="43">
+        <v>3272.6966539804698</v>
+      </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="28"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="42"/>
+      <c r="C72" s="40">
+        <v>1.7070088911500001</v>
+      </c>
+      <c r="D72" s="40">
+        <v>55.752407066478</v>
+      </c>
+      <c r="E72" s="41">
+        <v>174.066398935249</v>
+      </c>
+      <c r="F72" s="43">
+        <v>4390.7022047564396</v>
+      </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="28"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="41"/>
-      <c r="F73" s="42"/>
+      <c r="C73" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="D73" s="40">
+        <v>279.13115608910198</v>
+      </c>
+      <c r="E73" s="41">
+        <v>4.8395579726709999</v>
+      </c>
+      <c r="F73" s="43">
+        <v>1959.5437880939301</v>
+      </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="28"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="41"/>
-      <c r="F74" s="42"/>
+      <c r="C74" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D74" s="40">
+        <v>231.19440780618501</v>
+      </c>
+      <c r="E74" s="41">
+        <v>274.20319000586699</v>
+      </c>
+      <c r="F74" s="43">
+        <v>2816.5380192216398</v>
+      </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="28"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="41"/>
-      <c r="F75" s="42"/>
+      <c r="C75" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D75" s="40">
+        <v>63.156492192507997</v>
+      </c>
+      <c r="E75" s="41">
+        <v>182.35477272065401</v>
+      </c>
+      <c r="F75" s="43">
+        <v>4523.76504867722</v>
+      </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="28"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="41"/>
-      <c r="F76" s="42"/>
+      <c r="C76" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D76" s="40">
+        <v>171.98933073845501</v>
+      </c>
+      <c r="E76" s="41">
+        <v>150.646987126959</v>
+      </c>
+      <c r="F76" s="43">
+        <v>2001.3611335364201</v>
+      </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="28"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="41"/>
-      <c r="F77" s="42"/>
+      <c r="C77" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D77" s="40">
+        <v>201.004195575523</v>
+      </c>
+      <c r="E77" s="41">
+        <v>203.82821363250599</v>
+      </c>
+      <c r="F77" s="43">
+        <v>1875.6411642042999</v>
+      </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="28"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="41"/>
-      <c r="F78" s="42"/>
+      <c r="C78" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D78" s="40">
+        <v>64.853745134050996</v>
+      </c>
+      <c r="E78" s="41">
+        <v>299.57965422119599</v>
+      </c>
+      <c r="F78" s="43">
+        <v>2253.8048977603198</v>
+      </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="28"/>
-      <c r="C79" s="40"/>
-      <c r="D79" s="40"/>
-      <c r="E79" s="41"/>
-      <c r="F79" s="42"/>
+      <c r="C79" s="40">
+        <v>101.879000324511</v>
+      </c>
+      <c r="D79" s="40">
+        <v>93.418789483572994</v>
+      </c>
+      <c r="E79" s="41">
+        <v>132.017320097896</v>
+      </c>
+      <c r="F79" s="43">
+        <v>4998.0473158856703</v>
+      </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="28"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="40"/>
-      <c r="E80" s="41"/>
-      <c r="F80" s="42"/>
+      <c r="C80" s="40">
+        <v>182.187607068067</v>
+      </c>
+      <c r="D80" s="40">
+        <v>220.089810402371</v>
+      </c>
+      <c r="E80" s="41">
+        <v>123.021124288831</v>
+      </c>
+      <c r="F80" s="43">
+        <v>572.09706963462804</v>
+      </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="28"/>
-      <c r="C81" s="40"/>
-      <c r="D81" s="40"/>
-      <c r="E81" s="41"/>
-      <c r="F81" s="42"/>
+      <c r="C81" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D81" s="40">
+        <v>54.558839518341003</v>
+      </c>
+      <c r="E81" s="41">
+        <v>99.442854451214998</v>
+      </c>
+      <c r="F81" s="43">
+        <v>3157.0846209750698</v>
+      </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="28"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="40"/>
-      <c r="E82" s="41"/>
-      <c r="F82" s="42"/>
+      <c r="C82" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D82" s="40">
+        <v>157.425506887561</v>
+      </c>
+      <c r="E82" s="41">
+        <v>68.097416101297995</v>
+      </c>
+      <c r="F82" s="43">
+        <v>3139.31357177473</v>
+      </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="28"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="40"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="42"/>
+      <c r="C83" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D83" s="40">
+        <v>28.640703112682999</v>
+      </c>
+      <c r="E83" s="41">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F83" s="43">
+        <v>5403.98954776336</v>
+      </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="28"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="41"/>
-      <c r="F84" s="42"/>
+      <c r="C84" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D84" s="40">
+        <v>74.879614645074994</v>
+      </c>
+      <c r="E84" s="41">
+        <v>120.601248525366</v>
+      </c>
+      <c r="F84" s="43">
+        <v>3382.5678702792302</v>
+      </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="28"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="41"/>
-      <c r="F85" s="42"/>
+      <c r="C85" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D85" s="40">
+        <v>119.175320902888</v>
+      </c>
+      <c r="E85" s="41">
+        <v>99.522924284861006</v>
+      </c>
+      <c r="F85" s="43">
+        <v>3949.2566508592099</v>
+      </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="28"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="41"/>
-      <c r="F86" s="42"/>
+      <c r="C86" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D86" s="40">
+        <v>238.78503109151401</v>
+      </c>
+      <c r="E86" s="41">
+        <v>100.946849817154</v>
+      </c>
+      <c r="F86" s="43">
+        <v>3287.01872485896</v>
+      </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="28"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="41"/>
-      <c r="F87" s="42"/>
+      <c r="C87" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D87" s="40">
+        <v>126.972315210313</v>
+      </c>
+      <c r="E87" s="41">
+        <v>58.207885526173001</v>
+      </c>
+      <c r="F87" s="43">
+        <v>4104.7926329915799</v>
+      </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="28"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="40"/>
-      <c r="E88" s="41"/>
-      <c r="F88" s="42"/>
+      <c r="C88" s="40">
+        <v>160.08967396922199</v>
+      </c>
+      <c r="D88" s="40">
+        <v>103.309014309432</v>
+      </c>
+      <c r="E88" s="41">
+        <v>23.706928886707001</v>
+      </c>
+      <c r="F88" s="43">
+        <v>3729.1285866571802</v>
+      </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="28"/>
-      <c r="C89" s="28"/>
-      <c r="D89" s="40"/>
-      <c r="E89" s="41"/>
-      <c r="F89" s="42"/>
+      <c r="C89" s="28">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D89" s="40">
+        <v>273.06233055393102</v>
+      </c>
+      <c r="E89" s="41">
+        <v>128.46159969558201</v>
+      </c>
+      <c r="F89" s="43">
+        <v>3277.1221393543301</v>
+      </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="40"/>
-      <c r="E90" s="41"/>
-      <c r="F90" s="42"/>
+      <c r="C90" s="28">
+        <v>21.789564018377</v>
+      </c>
+      <c r="D90" s="40">
+        <v>132.52447143319799</v>
+      </c>
+      <c r="E90" s="41">
+        <v>13.108718594983999</v>
+      </c>
+      <c r="F90" s="43">
+        <v>4264.2051652938499</v>
+      </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="28"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="40"/>
-      <c r="E91" s="41"/>
-      <c r="F91" s="42"/>
+      <c r="C91" s="28">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D91" s="40">
+        <v>115.753648862123</v>
+      </c>
+      <c r="E91" s="41">
+        <v>171.497036478935</v>
+      </c>
+      <c r="F91" s="43">
+        <v>2092.8129180015098</v>
+      </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="40"/>
-      <c r="E92" s="41"/>
-      <c r="F92" s="42"/>
+      <c r="C92" s="28">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D92" s="40">
+        <v>152.139948549964</v>
+      </c>
+      <c r="E92" s="41">
+        <v>304.89662509580802</v>
+      </c>
+      <c r="F92" s="43">
+        <v>4354.1924553790104</v>
+      </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="40"/>
-      <c r="E93" s="41"/>
-      <c r="F93" s="42"/>
+      <c r="C93" s="28">
+        <v>112.500862500324</v>
+      </c>
+      <c r="D93" s="40">
+        <v>482.45087853223799</v>
+      </c>
+      <c r="E93" s="41">
+        <v>275.60847246113099</v>
+      </c>
+      <c r="F93" s="43">
+        <v>1289.94031046489</v>
+      </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="40"/>
-      <c r="E94" s="41"/>
-      <c r="F94" s="42"/>
+      <c r="C94" s="28">
+        <v>11.602086059326</v>
+      </c>
+      <c r="D94" s="40">
+        <v>37.699815808903999</v>
+      </c>
+      <c r="E94" s="41">
+        <v>267.05854666033503</v>
+      </c>
+      <c r="F94" s="43">
+        <v>5218.0755073747596</v>
+      </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="40"/>
-      <c r="E95" s="41"/>
-      <c r="F95" s="42"/>
+      <c r="C95" s="28">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D95" s="40">
+        <v>126.538864944913</v>
+      </c>
+      <c r="E95" s="41">
+        <v>119.057040688097</v>
+      </c>
+      <c r="F95" s="43">
+        <v>4587.9573233677602</v>
+      </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="40"/>
-      <c r="E96" s="41"/>
-      <c r="F96" s="42"/>
+      <c r="C96" s="28">
+        <v>97.788080912267006</v>
+      </c>
+      <c r="D96" s="40">
+        <v>54.55568008046</v>
+      </c>
+      <c r="E96" s="41">
+        <v>122.210372524044</v>
+      </c>
+      <c r="F96" s="43">
+        <v>2304.0162693849502</v>
+      </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="28"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="40"/>
-      <c r="E97" s="41"/>
-      <c r="F97" s="42"/>
+      <c r="C97" s="28">
+        <v>196.729593490806</v>
+      </c>
+      <c r="D97" s="40">
+        <v>50.125544825131001</v>
+      </c>
+      <c r="E97" s="41">
+        <v>236.597754564827</v>
+      </c>
+      <c r="F97" s="43">
+        <v>5571.7117639563703</v>
+      </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="40"/>
-      <c r="E98" s="41"/>
-      <c r="F98" s="42"/>
+      <c r="C98" s="28">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D98" s="40">
+        <v>54.512139406551</v>
+      </c>
+      <c r="E98" s="41">
+        <v>1.8300000000059999</v>
+      </c>
+      <c r="F98" s="43">
+        <v>4174.7324031058797</v>
+      </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="28"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="40"/>
-      <c r="E99" s="41"/>
-      <c r="F99" s="42"/>
+      <c r="C99" s="28">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D99" s="40">
+        <v>168.59346917802</v>
+      </c>
+      <c r="E99" s="41">
+        <v>354.30661885621799</v>
+      </c>
+      <c r="F99" s="43">
+        <v>4886.78390264274</v>
+      </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="40"/>
-      <c r="E100" s="41"/>
-      <c r="F100" s="42"/>
+      <c r="C100" s="28">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="D100" s="40">
+        <v>134.78976177774899</v>
+      </c>
+      <c r="E100" s="41">
+        <v>203.84633882647199</v>
+      </c>
+      <c r="F100" s="43">
+        <v>1694.8168950829099</v>
+      </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="28"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="40"/>
-      <c r="E101" s="41"/>
-      <c r="F101" s="42"/>
+      <c r="C101" s="28">
+        <v>119.95006219828601</v>
+      </c>
+      <c r="D101" s="40">
+        <v>169.33559647299501</v>
+      </c>
+      <c r="E101" s="41">
+        <v>319.30986083003398</v>
+      </c>
+      <c r="F101" s="43">
+        <v>4627.65229760486</v>
+      </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="28"/>

</xml_diff>